<commit_message>
Adding init to templates folder
</commit_message>
<xml_diff>
--- a/Instrument_Batch_1.xlsx
+++ b/Instrument_Batch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gerrydevine\dev\python\pids\instruments\unsw_pidinst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4379074-15D1-4664-9384-D6CF9806B637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6207F2C7-4BEC-4679-B3DE-E2ED368C4EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15750" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{5E038AFC-71DD-4F4A-BB94-645D0AA5BCD8}"/>
+    <workbookView xWindow="13050" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5E038AFC-71DD-4F4A-BB94-645D0AA5BCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -124,21 +124,6 @@
   </si>
   <si>
     <t>Model</t>
-  </si>
-  <si>
-    <r>
-      <t>Thermo Scientific ST 16 Centrifuge</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>The Sorvall™ ST 16 Centrifuge is designed for general-purpose laboratory applications, offering versatility and reliability for routine sample processing. It accommodates a variety of rotors and adapters, enabling compatibility with different tube types and sizes. Key features include:
@@ -253,6 +238,27 @@
   </si>
   <si>
     <t>Alternate_Identifier_Type</t>
+  </si>
+  <si>
+    <t>Date_Value</t>
+  </si>
+  <si>
+    <t>Date_Type</t>
+  </si>
+  <si>
+    <t>Commissioned</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>https://www.analytical.unsw.edu.au/facilities/emu</t>
+  </si>
+  <si>
+    <t>1|2|3</t>
+  </si>
+  <si>
+    <t>Thermo Scientific XP 12 Centrifuge.</t>
   </si>
 </sst>
 </file>
@@ -336,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,6 +371,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -703,7 +714,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,30 +746,30 @@
         <v>26</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="I1" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -767,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -807,19 +818,19 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,16 +903,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,13 +920,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -966,13 +977,13 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,10 +991,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1018,13 +1029,13 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="7"/>
     </row>
@@ -1049,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35D206A-6548-464A-8820-EB08CA68881B}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,16 +1079,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,21 +1113,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{53BFF732-2E10-4D85-AD07-8A9D25829FE1}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{FE03996D-7ABA-4B9D-BF66-7894D9FF80E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1143,10 +1172,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -1156,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1169,12 +1198,42 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE27CF6-4CC9-414C-B4E8-569DF508B397}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>44659</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>